<commit_message>
Photos and change on the gradio code.
</commit_message>
<xml_diff>
--- a/Feature Data.xlsx
+++ b/Feature Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stajyer\Documents\GitHub\milling-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80A5481-8EFE-4B4F-9F84-037C35EB3A44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7601B25-F4CE-44FF-A761-F0C73D589C84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{67E0F688-C1AF-42C8-9D95-4B3A27CBFA27}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E5264A-4086-46D9-8AD8-B7539128CB63}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1942,10 +1942,10 @@
         <v>0.83849499999999999</v>
       </c>
       <c r="E49" s="1">
+        <v>0.87033700000000003</v>
+      </c>
+      <c r="F49" s="1">
         <v>0.81776899999999997</v>
-      </c>
-      <c r="F49" s="1">
-        <v>3.5595000000000002E-2</v>
       </c>
       <c r="G49" s="1">
         <v>3.5595000000000002E-2</v>

</xml_diff>